<commit_message>
added feature and steps
</commit_message>
<xml_diff>
--- a/miscellaneous/User Stories.xlsx
+++ b/miscellaneous/User Stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonat\Desktop\Revature\Projects\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonat\Desktop\Revature\Projects\Project2\miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819F7CB2-B4FC-4FCD-A992-AC204427779F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3566596F-D04F-44E9-AF40-20FA12C96193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="870" windowWidth="27105" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="129">
   <si>
     <t>As a…</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Given the admin is on admin page</t>
   </si>
   <si>
-    <t>When the admin clicks on users</t>
-  </si>
-  <si>
     <t>When the admin clicks delete user</t>
   </si>
   <si>
@@ -363,45 +360,18 @@
     <t>Scenario: As an user, I want to search other users using their name</t>
   </si>
   <si>
-    <t xml:space="preserve">Given the user is on any page </t>
-  </si>
-  <si>
-    <t>Given the user is on any page</t>
-  </si>
-  <si>
-    <t>When the user enter other user's first name and last name on the search bar</t>
-  </si>
-  <si>
-    <t>When the user click search button</t>
-  </si>
-  <si>
     <t>Then the user should see the searched user's name and a link to their profile</t>
   </si>
   <si>
     <t>Scenario: As an user, I want to view my profile</t>
   </si>
   <si>
-    <t>Given the user is on their homepage</t>
-  </si>
-  <si>
-    <t>When the user click on the My Profile link</t>
-  </si>
-  <si>
     <t>Then the user should be redirect to their profile page</t>
   </si>
   <si>
     <t>Scenario: As an user, I want to view other profiles</t>
   </si>
   <si>
-    <t>When the user click on the search button</t>
-  </si>
-  <si>
-    <t>When the user see the searched user's name and a link to their profile</t>
-  </si>
-  <si>
-    <t>When the user click on the link</t>
-  </si>
-  <si>
     <t>Then the user should be redirected to the searched user's profile page</t>
   </si>
   <si>
@@ -417,16 +387,31 @@
     <t>When the user click on the follow button</t>
   </si>
   <si>
-    <t>Then the user should now followed and the follow button should change to unfollow</t>
-  </si>
-  <si>
     <t>Scenario: As an user, I want to unfollow other users</t>
   </si>
   <si>
-    <t>When the user click on the unfollow button</t>
-  </si>
-  <si>
-    <t>Then the user should now unfollowed and the unfollow button should change to follow</t>
+    <t>When the user clicks on the searched person</t>
+  </si>
+  <si>
+    <t>When the user clicks search button</t>
+  </si>
+  <si>
+    <t>When the user enters other user's first name on the search bar</t>
+  </si>
+  <si>
+    <t>When the user clicks on the My Profile button</t>
+  </si>
+  <si>
+    <t>When the user clicks on the unfollow button</t>
+  </si>
+  <si>
+    <t>Then the user should now be followed and the follow button should change to unfollow</t>
+  </si>
+  <si>
+    <t>Then the user should now be unfollowed and the unfollow button should change to follow</t>
+  </si>
+  <si>
+    <t>Feature:  As an admin I want to log in, and log out</t>
   </si>
 </sst>
 </file>
@@ -728,21 +713,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -752,13 +737,13 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E133"/>
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1078,13 +1063,13 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="19" t="s">
@@ -1223,13 +1208,13 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="34"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="19" t="s">
@@ -1431,13 +1416,13 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="26"/>
+      <c r="A61" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="34"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="19" t="s">
@@ -1450,22 +1435,22 @@
         <v>33</v>
       </c>
       <c r="E62" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="E63" s="15" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="E64" s="16" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="E65" s="16" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1473,7 +1458,7 @@
         <v>68</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1487,22 +1472,22 @@
         <v>31</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="E69" s="15" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="E70" s="16" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="E71" s="18" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1516,42 +1501,42 @@
         <v>32</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="E74" s="15" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="E75" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="E76" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="E77" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="E78" s="18" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="26"/>
+      <c r="A80" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="34"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="19" t="s">
@@ -1564,22 +1549,22 @@
         <v>30</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="E82" s="15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="E83" s="16" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="E84" s="18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1593,41 +1578,41 @@
         <v>28</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="E87" s="15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="E88" s="16" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="E89" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="24" t="s">
+      <c r="A91" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="26"/>
+      <c r="B91" s="33"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="34"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="32" t="s">
+      <c r="A92" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B92" s="33" t="s">
+      <c r="B92" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C92" s="34" t="s">
+      <c r="C92" s="28" t="s">
         <v>35</v>
       </c>
       <c r="E92" s="22" t="s">
@@ -1645,7 +1630,7 @@
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="18" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1653,11 +1638,8 @@
       <c r="C96" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="E96" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" s="8" t="s">
         <v>3</v>
       </c>
@@ -1668,33 +1650,33 @@
         <v>36</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="E99" s="15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:6">
       <c r="E100" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="E101" s="16" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
-      <c r="E101" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:6">
       <c r="C102" s="23" t="s">
         <v>68</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" s="8" t="s">
         <v>3</v>
       </c>
@@ -1705,38 +1687,47 @@
         <v>37</v>
       </c>
       <c r="E104" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="E105" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
-      <c r="E105" s="15" t="s">
+    <row r="106" spans="1:6">
+      <c r="E106" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="E107" s="16" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
-      <c r="E106" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="E107" s="16" t="s">
+    <row r="108" spans="1:6">
+      <c r="E108" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
-      <c r="E108" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:6">
       <c r="C109" s="23" t="s">
         <v>68</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="B110" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="C110" s="33"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="33"/>
+      <c r="F110" s="34"/>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" s="8" t="s">
         <v>3</v>
       </c>
@@ -1747,27 +1738,27 @@
         <v>40</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="E112" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="E113" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="E114" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="E115" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -1781,7 +1772,7 @@
         <v>26</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -1789,22 +1780,22 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="E118" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="E119" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="E120" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B129" s="30"/>
       <c r="C129" s="30"/>
@@ -1812,10 +1803,10 @@
       <c r="E129" s="31"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="27" t="s">
+      <c r="A130" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="B130" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C130" s="21" t="s">
@@ -1838,10 +1829,10 @@
         <v>4</v>
       </c>
       <c r="B132" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C132" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C132" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -1856,13 +1847,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A129:E129"/>
     <mergeCell ref="A80:E80"/>
     <mergeCell ref="A91:E91"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A61:E61"/>
+    <mergeCell ref="B110:F110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>